<commit_message>
added multi figure plotting for 1D uncertainty
</commit_message>
<xml_diff>
--- a/paper_plots_and_data/table_results.xlsx
+++ b/paper_plots_and_data/table_results.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="7scenes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="kitti" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="kitti_nll" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="1d_supp" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t xml:space="preserve">Error</t>
   </si>
@@ -111,17 +113,51 @@
   </si>
   <si>
     <t xml:space="preserve">UnDeepVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activation Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropout (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HydraNet (no direct uncertainty)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -142,11 +178,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,8 +222,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,7 +239,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,153 +268,153 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>6.3</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>-6</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>14.9</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>11.3</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>-3.6</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>14.3</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>-3.9</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>8.6</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>5.6</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>-5.4</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>4.8</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>8.8</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>5.4</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>11.8</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>12.4</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>-4.7</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -399,399 +434,432 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="0"/>
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="n">
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="n">
         <v>65.27</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="2" t="n">
         <v>6.23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="0"/>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="n">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="n">
         <v>4.14</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="2" t="n">
         <v>1.92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="A8" s="0"/>
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>27.9138160337396</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="3" t="n">
         <v>6.25385179420857</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>1.96338401432886</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="2" t="n">
         <v>0.80716078142071</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="0"/>
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="3" t="n">
         <v>9.85720084641496</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="3" t="n">
         <v>2.82812607258089</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <v>1.33797194313331</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>0.628394162194651</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="A10" s="0"/>
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>12.41</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>2.45</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>1.28</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="2" t="n">
         <v>0.542</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="A14" s="0"/>
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="n">
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="n">
         <v>57.59</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="2" t="n">
         <v>4.09</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="0"/>
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="n">
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="n">
         <v>5.58</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" s="2" t="n">
         <v>2.44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="0"/>
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="2" t="n">
         <v>64.6652075654143</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="D17" s="2" t="n">
         <v>8.44709778306827</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="2" t="n">
         <v>1.47417830906299</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" s="2" t="n">
         <v>0.558778072134629</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="A18" s="0"/>
+      <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="3" t="n">
         <v>50.1859710229814</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="3" t="n">
         <v>6.50564039179401</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="3" t="n">
         <v>1.46686305161936</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="3" t="n">
         <v>0.631285701246831</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+      <c r="A19" s="0"/>
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="2" t="n">
         <v>16.33</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D19" s="2" t="n">
         <v>3.19</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="2" t="n">
         <v>1.21</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" s="2" t="n">
         <v>0.467</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="1" t="n">
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2" t="n">
         <v>2.62</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="2" t="n">
         <v>3.61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="1" t="n">
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2" t="n">
         <v>16.76</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22" s="2" t="n">
         <v>4.06</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="1" t="n">
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2" t="n">
         <v>3.4</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23" s="2" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="3" t="n">
         <v>23.7178817517014</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="3" t="n">
         <v>8.10466315648884</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="2" t="n">
         <v>1.79093039741156</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" s="2" t="n">
         <v>0.78975279517017</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="3" t="n">
         <v>9.85074248332791</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="3" t="n">
         <v>3.2310535841306</v>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="3" t="n">
         <v>1.38400618111673</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="3" t="n">
         <v>0.603270351455262</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="2" t="n">
         <v>5.83</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="2" t="n">
         <v>2.05</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="2" t="n">
         <v>0.69</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="2" t="n">
         <v>0.32</v>
       </c>
     </row>
@@ -804,4 +872,308 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>0.0476711853057013</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>-16.843542</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>0.131946651486356</v>
+      </c>
+      <c r="D3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>0.0882300274168881</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0.199439520665701</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0.0425987687119114</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>-18.441093</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0.0706503414434783</v>
+      </c>
+      <c r="D8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>0.079626885910861</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0.137778681739281</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0.032600828357014</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>-19.313206</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>0.0641467400436564</v>
+      </c>
+      <c r="D13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>0.0581712608629401</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>0.108623168490447</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="18.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
re-added 1D noise results
</commit_message>
<xml_diff>
--- a/paper_plots_and_data/table_results.xlsx
+++ b/paper_plots_and_data/table_results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t xml:space="preserve">Error</t>
   </si>
@@ -124,10 +124,10 @@
     <t xml:space="preserve">Uncertainty Method</t>
   </si>
   <si>
-    <t xml:space="preserve"># layers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activation Layer</t>
+    <t xml:space="preserve">Learning Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Momentum</t>
   </si>
   <si>
     <t xml:space="preserve">Dropout (%)</t>
@@ -136,10 +136,7 @@
     <t xml:space="preserve">Dropout</t>
   </si>
   <si>
-    <t xml:space="preserve">SELU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct</t>
+    <t xml:space="preserve">Direct Regression</t>
   </si>
   <si>
     <t xml:space="preserve">Bagging</t>
@@ -222,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,6 +237,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1060,16 +1061,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6938775510204"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="18.7551020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
@@ -1081,10 +1082,10 @@
       <c r="B1" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="0" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1093,63 +1094,54 @@
         <v>36</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>0.01</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>5</v>
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1158,12 +1150,12 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5</v>
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>